<commit_message>
Python: * Add xloJpyRun to execute arbtrary code on the kernel (needed to adjust the message parsing logic for this) * Improve xloJpyConnect so it can search all jupyter instances given a notebook name. * Added a few comments / updated docs
</commit_message>
<xml_diff>
--- a/tests/python/TestJupyter.xlsx
+++ b/tests/python/TestJupyter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\dev\xloil\tests\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A77B046-5AB0-4F71-9BBE-2F69306D3412}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664B8701-BA37-4AAA-AD1E-5212072720D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2136" yWindow="936" windowWidth="20136" windowHeight="10116" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -33,7 +27,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>kernel-69b9e5a2-977f-4ece-9f2f-5cda0579fdb0.json</t>
+    <t>TestJupyterConnection.ipynb</t>
   </si>
 </sst>
 </file>
@@ -99,28 +93,28 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="xloil.rtd.43242cb4.b0ae.47e3.b8b8.914fceef9a1e">
+    <main first="xloil.80c4bb32.56de.41f9.ab86.73f3295366ff">
       <tp>
         <v>0</v>
         <stp/>
-        <stp>153a54bc-780ccdcca77b26dc2c3d8a83_watch_var</stp>
-        <tr r="D5" s="1"/>
-        <tr r="D7" s="1"/>
-        <tr r="B7" s="1"/>
-        <tr r="D6" s="1"/>
-        <tr r="B6" s="1"/>
-        <tr r="C7" s="1"/>
-        <tr r="C5" s="1"/>
-        <tr r="C6" s="1"/>
-        <tr r="B5" s="1"/>
+        <stp>kernel-45cd273f-f93c-435d-ae47-29ae997b41ff.json</stp>
+        <tr r="B3" s="1"/>
       </tp>
     </main>
-    <main first="xloil.rtd.0b1c1bc7.454a.4de6.944d.276087bfb6c7">
+    <main first="xloil.80c4bb32.56de.41f9.ab86.73f3295366ff">
       <tp>
         <v>0</v>
         <stp/>
-        <stp>{848AE3EA-82FC-4BA8-BF87-42B1EAE0897A}</stp>
-        <tr r="B3" s="1"/>
+        <stp>427ea3a4-84e2dbe69b392c72ea7f25d4_watch_var</stp>
+        <tr r="C6" s="1"/>
+        <tr r="C5" s="1"/>
+        <tr r="D7" s="1"/>
+        <tr r="B5" s="1"/>
+        <tr r="B6" s="1"/>
+        <tr r="C7" s="1"/>
+        <tr r="D6" s="1"/>
+        <tr r="B7" s="1"/>
+        <tr r="D5" s="1"/>
       </tp>
     </main>
   </volType>
@@ -424,69 +418,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D10"/>
+  <dimension ref="B2:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="7" max="7" width="15" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:7">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:7">
       <c r="B3" t="str">
         <f>_xll.xloJpyConnect(B2)</f>
-        <v>欣[TestJupyter.xlsx]Sheet1!R3C2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5" t="e">
-        <f t="array" ref="B5:D7">_xll.xloJpyWatch("watch_var",B3)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D5" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D6" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C7" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D7" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4">
+        <v>欣[TestJupyter.xlsx]Sheet1!R3C2,A</v>
+      </c>
+      <c r="G3">
+        <f>_xll.xloJpyRun(B3,"func2({})", 7)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5">
+        <f t="array" ref="B5:D7">_xll.xloJpyWatch(B3,"watch_var")</f>
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
       <c r="B9" t="e">
-        <f>_xll.jptest(1)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10" t="e">
-        <f>_xll.xloLog()</f>
-        <v>#N/A</v>
+        <f ca="1">_xll.jptest(1)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="E13" t="str">
+        <f>_xll.xloPyDebug("pdb")</f>
+        <v>pdb</v>
       </c>
     </row>
   </sheetData>

</xml_diff>